<commit_message>
run test and add note on read me
</commit_message>
<xml_diff>
--- a/outfile/your_report.xlsx
+++ b/outfile/your_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
   <si>
     <t>Summary</t>
   </si>
@@ -190,91 +190,85 @@
     <t>Coef Correlation between Categorical variables and a chosen target variable</t>
   </si>
   <si>
-    <t>Instruction Date_2019-12-19</t>
-  </si>
-  <si>
-    <t>Instruction Date_2016-07-09</t>
-  </si>
-  <si>
-    <t>Instruction Date_2017-01-13</t>
-  </si>
-  <si>
-    <t>BIC FI Destination_ROYCCAT2</t>
-  </si>
-  <si>
-    <t>Instruction Date_2015-12-05</t>
-  </si>
-  <si>
-    <t>BIC FI Initiation_BARCGB5G</t>
-  </si>
-  <si>
-    <t>Instruction Date_2015-07-27</t>
-  </si>
-  <si>
-    <t>Format Expedied_MT205</t>
-  </si>
-  <si>
-    <t>BIC Receiver_BNDCCAMMXIN</t>
-  </si>
-  <si>
-    <t>BIC FI Destination_CHASUS33</t>
-  </si>
-  <si>
-    <t>BIC Receiver_ROYCCAT2</t>
-  </si>
-  <si>
-    <t>BIC FI Initiation_BNDCCAMMINT</t>
-  </si>
-  <si>
-    <t>BIC Sender_BNDCCAMMINT</t>
-  </si>
-  <si>
-    <t>Instruction Date_2019-08-24</t>
+    <t>Instruction Date_2020-02-27</t>
+  </si>
+  <si>
+    <t>BIC FI Initiation_CHASUS33FXR</t>
+  </si>
+  <si>
+    <t>Instruction Date_2014-11-20</t>
+  </si>
+  <si>
+    <t>BIC FI Initiation_ROYCGB2L</t>
+  </si>
+  <si>
+    <t>Instruction Date_2015-10-21</t>
+  </si>
+  <si>
+    <t>BIC Sender_ROYCCAT2</t>
+  </si>
+  <si>
+    <t>Instruction Date_2018-07-15</t>
+  </si>
+  <si>
+    <t>BIC FI Initiation_ROYCCAT2</t>
+  </si>
+  <si>
+    <t>Instruction Date_2016-09-17</t>
+  </si>
+  <si>
+    <t>BIC FI Destination_BNDCCAMMINT</t>
   </si>
   <si>
     <t>ind_lvts_Oui</t>
   </si>
   <si>
-    <t>Clients_Treasury</t>
-  </si>
-  <si>
-    <t>BIC Receiver_CIBCCATTXXX</t>
-  </si>
-  <si>
-    <t>Instruction Date_2016-01-18</t>
-  </si>
-  <si>
-    <t>Instruction Date_2014-08-29</t>
-  </si>
-  <si>
-    <t>Network Transmission Recieved_Interac</t>
+    <t>Instruction Date_2020-02-26</t>
+  </si>
+  <si>
+    <t>Country Sender_CA</t>
+  </si>
+  <si>
+    <t>Country FI Initiation_CA</t>
+  </si>
+  <si>
+    <t>BIC FI Initiation_BNDCCAMM</t>
+  </si>
+  <si>
+    <t>is_sender FI Initiation_Oui</t>
+  </si>
+  <si>
+    <t>Channel_UNKNOWN</t>
+  </si>
+  <si>
+    <t>BIC Sender_BCANCAW2</t>
+  </si>
+  <si>
+    <t>BIC FI Initiation_BCANCAW2</t>
+  </si>
+  <si>
+    <t>Instruction Date_2014-12-27</t>
+  </si>
+  <si>
+    <t>Instruction Date_2018-01-26</t>
+  </si>
+  <si>
+    <t>Solution_Product_Direct_Debit</t>
+  </si>
+  <si>
+    <t>Instruction_Withdrawal</t>
+  </si>
+  <si>
+    <t>Instruction Date_2017-07-11</t>
   </si>
   <si>
     <t>Country FI Initiation_GB</t>
   </si>
   <si>
-    <t>BIC FI Initiation_BNDCCAMMIMM</t>
-  </si>
-  <si>
-    <t>Instruction Date_2019-11-03</t>
-  </si>
-  <si>
-    <t>BIC FI Initiation_BOFMCAT2FXM</t>
-  </si>
-  <si>
-    <t>Instruction Date_2017-06-11</t>
-  </si>
-  <si>
-    <t>Instruction Date_2017-06-14</t>
-  </si>
-  <si>
-    <t>Instruction Date_2018-05-02</t>
-  </si>
-  <si>
-    <t>Instruction Date_2015-02-17</t>
-  </si>
-  <si>
-    <t>Network Transmission Expedied_Swift - Fin (SAA)</t>
+    <t>Country FI Initiation_US</t>
+  </si>
+  <si>
+    <t>Instruction Date_2020-01-26</t>
   </si>
 </sst>
 </file>
@@ -1682,10 +1676,10 @@
         <v>1</v>
       </c>
       <c r="C46">
-        <v>0.02967314703415103</v>
+        <v>0.04375210694513654</v>
       </c>
       <c r="D46">
-        <v>0.9829162607688804</v>
+        <v>0.9823871556748695</v>
       </c>
     </row>
     <row r="47" spans="1:30">
@@ -1693,13 +1687,13 @@
         <v>24</v>
       </c>
       <c r="B47">
-        <v>0.02967314703415103</v>
+        <v>0.04375210694513654</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>0.02710588260357007</v>
+        <v>0.05271375803118115</v>
       </c>
     </row>
     <row r="48" spans="1:30">
@@ -1707,10 +1701,10 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>0.9829162607688804</v>
+        <v>0.9823871556748695</v>
       </c>
       <c r="C48">
-        <v>0.02710588260357007</v>
+        <v>0.05271375803118115</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1739,7 +1733,7 @@
         <v>58</v>
       </c>
       <c r="B57">
-        <v>0.61</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1747,7 +1741,7 @@
         <v>59</v>
       </c>
       <c r="B58">
-        <v>0.53</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1755,7 +1749,7 @@
         <v>60</v>
       </c>
       <c r="B59">
-        <v>0.3</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1763,7 +1757,7 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>0.26</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1771,7 +1765,7 @@
         <v>62</v>
       </c>
       <c r="B61">
-        <v>0.24</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1779,7 +1773,7 @@
         <v>63</v>
       </c>
       <c r="B62">
-        <v>0.21</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1787,7 +1781,7 @@
         <v>64</v>
       </c>
       <c r="B63">
-        <v>0.21</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1795,7 +1789,7 @@
         <v>65</v>
       </c>
       <c r="B64">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1803,7 +1797,7 @@
         <v>66</v>
       </c>
       <c r="B65">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1811,7 +1805,7 @@
         <v>67</v>
       </c>
       <c r="B66">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1819,7 +1813,7 @@
         <v>68</v>
       </c>
       <c r="B67">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1827,7 +1821,7 @@
         <v>69</v>
       </c>
       <c r="B68">
-        <v>0.14</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1835,7 +1829,7 @@
         <v>70</v>
       </c>
       <c r="B69">
-        <v>0.13</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1843,7 +1837,7 @@
         <v>71</v>
       </c>
       <c r="B70">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1851,7 +1845,7 @@
         <v>72</v>
       </c>
       <c r="B71">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1859,7 +1853,7 @@
         <v>73</v>
       </c>
       <c r="B72">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1867,7 +1861,7 @@
         <v>74</v>
       </c>
       <c r="B73">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1875,7 +1869,7 @@
         <v>75</v>
       </c>
       <c r="B74">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1883,7 +1877,7 @@
         <v>76</v>
       </c>
       <c r="B75">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1891,7 +1885,7 @@
         <v>77</v>
       </c>
       <c r="B76">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1899,7 +1893,7 @@
         <v>78</v>
       </c>
       <c r="B77">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1907,7 +1901,7 @@
         <v>79</v>
       </c>
       <c r="B78">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1915,12 +1909,12 @@
         <v>80</v>
       </c>
       <c r="B79">
-        <v>0.05</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="B80">
         <v>0.05</v>
@@ -1928,7 +1922,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81">
         <v>0.05</v>
@@ -1936,7 +1930,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82">
         <v>0.05</v>
@@ -1944,23 +1938,23 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B83">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="B84">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B85">
         <v>0.04</v>

</xml_diff>

<commit_message>
completed fhandler.py and unittest for fhandler
</commit_message>
<xml_diff>
--- a/outfile/your_report.xlsx
+++ b/outfile/your_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="87">
   <si>
     <t>Summary</t>
   </si>
@@ -193,64 +193,73 @@
     <t>Instruction Date_2020-02-27</t>
   </si>
   <si>
+    <t>Instruction Date_2014-02-04</t>
+  </si>
+  <si>
+    <t>Instruction Date_2018-10-04</t>
+  </si>
+  <si>
+    <t>Instruction Date_2014-02-26</t>
+  </si>
+  <si>
+    <t>Country FI Initiation_CA</t>
+  </si>
+  <si>
+    <t>Instruction Date_2014-07-14</t>
+  </si>
+  <si>
+    <t>is_sender FI Initiation_Oui</t>
+  </si>
+  <si>
+    <t>ind_lvts_Oui</t>
+  </si>
+  <si>
+    <t>Country Sender_CA</t>
+  </si>
+  <si>
+    <t>BIC FI Initiation_TDOMCATTTOR</t>
+  </si>
+  <si>
+    <t>BIC FI Initiation_ROYCCAT2</t>
+  </si>
+  <si>
+    <t>BIC FI Destination_ROYCCAT2</t>
+  </si>
+  <si>
     <t>BIC FI Initiation_CHASUS33FXR</t>
   </si>
   <si>
-    <t>Instruction Date_2014-11-20</t>
-  </si>
-  <si>
-    <t>BIC FI Initiation_ROYCGB2L</t>
-  </si>
-  <si>
-    <t>Instruction Date_2015-10-21</t>
+    <t>BIC Sender_TDOMCATTTOR</t>
   </si>
   <si>
     <t>BIC Sender_ROYCCAT2</t>
   </si>
   <si>
-    <t>Instruction Date_2018-07-15</t>
-  </si>
-  <si>
-    <t>BIC FI Initiation_ROYCCAT2</t>
-  </si>
-  <si>
-    <t>Instruction Date_2016-09-17</t>
-  </si>
-  <si>
-    <t>BIC FI Destination_BNDCCAMMINT</t>
-  </si>
-  <si>
-    <t>ind_lvts_Oui</t>
-  </si>
-  <si>
-    <t>Instruction Date_2020-02-26</t>
-  </si>
-  <si>
-    <t>Country Sender_CA</t>
-  </si>
-  <si>
-    <t>Country FI Initiation_CA</t>
+    <t>Channel_UNKNOWN</t>
+  </si>
+  <si>
+    <t>Instruction Date_2016-02-15</t>
+  </si>
+  <si>
+    <t>BIC FI Initiation_HKBCCATT</t>
+  </si>
+  <si>
+    <t>BIC Sender_ROYCCAT3IMM</t>
+  </si>
+  <si>
+    <t>BIC FI Initiation_ROYCCAT3IMM</t>
+  </si>
+  <si>
+    <t>Instruction Date_2014-06-17</t>
   </si>
   <si>
     <t>BIC FI Initiation_BNDCCAMM</t>
   </si>
   <si>
-    <t>is_sender FI Initiation_Oui</t>
-  </si>
-  <si>
-    <t>Channel_UNKNOWN</t>
-  </si>
-  <si>
-    <t>BIC Sender_BCANCAW2</t>
-  </si>
-  <si>
-    <t>BIC FI Initiation_BCANCAW2</t>
-  </si>
-  <si>
-    <t>Instruction Date_2014-12-27</t>
-  </si>
-  <si>
-    <t>Instruction Date_2018-01-26</t>
+    <t>BIC Sender_HKBCCATT</t>
+  </si>
+  <si>
+    <t>Clients_Institutionnal</t>
   </si>
   <si>
     <t>Solution_Product_Direct_Debit</t>
@@ -259,16 +268,13 @@
     <t>Instruction_Withdrawal</t>
   </si>
   <si>
-    <t>Instruction Date_2017-07-11</t>
-  </si>
-  <si>
-    <t>Country FI Initiation_GB</t>
-  </si>
-  <si>
-    <t>Country FI Initiation_US</t>
-  </si>
-  <si>
-    <t>Instruction Date_2020-01-26</t>
+    <t>Instruction Date_2018-05-09</t>
+  </si>
+  <si>
+    <t>Payment Engine_System 2</t>
+  </si>
+  <si>
+    <t>Instruction Date_2014-07-31</t>
   </si>
 </sst>
 </file>
@@ -1676,10 +1682,10 @@
         <v>1</v>
       </c>
       <c r="C46">
-        <v>0.04375210694513654</v>
+        <v>-0.005968836144085329</v>
       </c>
       <c r="D46">
-        <v>0.9823871556748695</v>
+        <v>0.982716182458989</v>
       </c>
     </row>
     <row r="47" spans="1:30">
@@ -1687,13 +1693,13 @@
         <v>24</v>
       </c>
       <c r="B47">
-        <v>0.04375210694513654</v>
+        <v>-0.005968836144085329</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>0.05271375803118115</v>
+        <v>0.01184095356250245</v>
       </c>
     </row>
     <row r="48" spans="1:30">
@@ -1701,10 +1707,10 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>0.9823871556748695</v>
+        <v>0.982716182458989</v>
       </c>
       <c r="C48">
-        <v>0.05271375803118115</v>
+        <v>0.01184095356250245</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1733,7 +1739,7 @@
         <v>58</v>
       </c>
       <c r="B57">
-        <v>0.92</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1741,7 +1747,7 @@
         <v>59</v>
       </c>
       <c r="B58">
-        <v>0.21</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1749,7 +1755,7 @@
         <v>60</v>
       </c>
       <c r="B59">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1757,7 +1763,7 @@
         <v>61</v>
       </c>
       <c r="B60">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1765,7 +1771,7 @@
         <v>62</v>
       </c>
       <c r="B61">
-        <v>0.16</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1773,7 +1779,7 @@
         <v>63</v>
       </c>
       <c r="B62">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1781,7 +1787,7 @@
         <v>64</v>
       </c>
       <c r="B63">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1813,7 +1819,7 @@
         <v>68</v>
       </c>
       <c r="B67">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1821,7 +1827,7 @@
         <v>69</v>
       </c>
       <c r="B68">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1877,7 +1883,7 @@
         <v>76</v>
       </c>
       <c r="B75">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1885,7 +1891,7 @@
         <v>77</v>
       </c>
       <c r="B76">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1893,7 +1899,7 @@
         <v>78</v>
       </c>
       <c r="B77">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1901,7 +1907,7 @@
         <v>79</v>
       </c>
       <c r="B78">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1909,12 +1915,12 @@
         <v>80</v>
       </c>
       <c r="B79">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="B80">
         <v>0.05</v>
@@ -1922,23 +1928,23 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B81">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B82">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B83">
         <v>0.04</v>
@@ -1946,7 +1952,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="B84">
         <v>0.04</v>
@@ -1954,7 +1960,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B85">
         <v>0.04</v>

</xml_diff>